<commit_message>
Started on vignette for figure 3. Added box_stats functions from lmisc to package to prevent dependence on lmisc
</commit_message>
<xml_diff>
--- a/inst/extdata/main-results.xlsx
+++ b/inst/extdata/main-results.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lestes/Dropbox/publications/ecoscales/inst/extdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="180" windowWidth="25040" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="25040" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -39282,6 +39290,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -40958,15 +40971,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W351"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E185" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="Q1" sqref="Q1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A246" sqref="A246:W351"/>
-      <selection pane="bottomRight" activeCell="J178" sqref="J178"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" style="36" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" style="36" customWidth="1"/>
@@ -40991,7 +41004,7 @@
     <col min="24" max="16384" width="10.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" s="30" t="s">
         <v>268</v>
       </c>
@@ -41062,7 +41075,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>288</v>
       </c>
@@ -41138,7 +41151,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>288</v>
       </c>
@@ -41214,7 +41227,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>288</v>
       </c>
@@ -41290,7 +41303,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>288</v>
       </c>
@@ -41366,7 +41379,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>288</v>
       </c>
@@ -41442,7 +41455,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>288</v>
       </c>
@@ -41515,7 +41528,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>288</v>
       </c>
@@ -41588,7 +41601,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>288</v>
       </c>
@@ -41662,7 +41675,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>288</v>
       </c>
@@ -41736,7 +41749,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>288</v>
       </c>
@@ -41810,7 +41823,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>288</v>
       </c>
@@ -41884,7 +41897,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
         <v>288</v>
       </c>
@@ -41959,7 +41972,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
         <v>288</v>
       </c>
@@ -42034,7 +42047,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
         <v>288</v>
       </c>
@@ -42108,7 +42121,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>288</v>
       </c>
@@ -42182,7 +42195,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>288</v>
       </c>
@@ -42255,7 +42268,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
         <v>288</v>
       </c>
@@ -42328,7 +42341,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>288</v>
       </c>
@@ -42402,7 +42415,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A20" s="46" t="s">
         <v>288</v>
       </c>
@@ -42474,7 +42487,7 @@
       </c>
       <c r="W20" s="47"/>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
         <v>288</v>
       </c>
@@ -42548,7 +42561,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
         <v>288</v>
       </c>
@@ -42621,7 +42634,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
         <v>288</v>
       </c>
@@ -42697,7 +42710,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>288</v>
       </c>
@@ -42774,7 +42787,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
         <v>288</v>
       </c>
@@ -42850,7 +42863,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>288</v>
       </c>
@@ -42927,7 +42940,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
         <v>288</v>
       </c>
@@ -43004,7 +43017,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A28" s="32" t="s">
         <v>288</v>
       </c>
@@ -43082,7 +43095,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A29" s="32" t="s">
         <v>288</v>
       </c>
@@ -43160,7 +43173,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A30" s="32" t="s">
         <v>288</v>
       </c>
@@ -43239,7 +43252,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A31" s="32" t="s">
         <v>288</v>
       </c>
@@ -43318,7 +43331,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A32" s="32" t="s">
         <v>288</v>
       </c>
@@ -43397,7 +43410,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A33" s="32" t="s">
         <v>288</v>
       </c>
@@ -43471,7 +43484,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A34" s="32" t="s">
         <v>288</v>
       </c>
@@ -43545,7 +43558,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A35" s="32" t="s">
         <v>288</v>
       </c>
@@ -43621,7 +43634,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A36" s="32" t="s">
         <v>288</v>
       </c>
@@ -43696,7 +43709,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A37" s="32" t="s">
         <v>288</v>
       </c>
@@ -43774,7 +43787,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A38" s="32" t="s">
         <v>288</v>
       </c>
@@ -43852,7 +43865,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A39" s="32" t="s">
         <v>288</v>
       </c>
@@ -43929,7 +43942,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A40" s="32" t="s">
         <v>288</v>
       </c>
@@ -44003,7 +44016,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A41" s="32" t="s">
         <v>288</v>
       </c>
@@ -44077,7 +44090,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A42" s="32" t="s">
         <v>288</v>
       </c>
@@ -44152,7 +44165,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A43" s="32" t="s">
         <v>288</v>
       </c>
@@ -44226,7 +44239,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A44" s="32" t="s">
         <v>288</v>
       </c>
@@ -44300,7 +44313,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A45" s="32" t="s">
         <v>288</v>
       </c>
@@ -44373,7 +44386,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A46" s="32" t="s">
         <v>288</v>
       </c>
@@ -44444,7 +44457,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A47" s="32" t="s">
         <v>288</v>
       </c>
@@ -44519,7 +44532,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A48" s="32" t="s">
         <v>288</v>
       </c>
@@ -44597,7 +44610,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A49" s="32" t="s">
         <v>288</v>
       </c>
@@ -44675,7 +44688,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A50" s="32" t="s">
         <v>288</v>
       </c>
@@ -44747,7 +44760,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A51" s="32" t="s">
         <v>288</v>
       </c>
@@ -44820,7 +44833,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A52" s="32" t="s">
         <v>288</v>
       </c>
@@ -44895,7 +44908,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A53" s="32" t="s">
         <v>288</v>
       </c>
@@ -44970,7 +44983,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A54" s="32" t="s">
         <v>288</v>
       </c>
@@ -45045,7 +45058,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A55" s="32" t="s">
         <v>288</v>
       </c>
@@ -45123,7 +45136,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A56" s="32" t="s">
         <v>288</v>
       </c>
@@ -45196,7 +45209,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A57" s="32" t="s">
         <v>288</v>
       </c>
@@ -45270,7 +45283,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A58" s="32" t="s">
         <v>288</v>
       </c>
@@ -45345,7 +45358,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A59" s="32" t="s">
         <v>288</v>
       </c>
@@ -45423,7 +45436,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A60" s="32" t="s">
         <v>288</v>
       </c>
@@ -45500,7 +45513,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A61" s="32" t="s">
         <v>288</v>
       </c>
@@ -45573,7 +45586,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A62" s="32" t="s">
         <v>288</v>
       </c>
@@ -45643,7 +45656,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A63" s="32" t="s">
         <v>288</v>
       </c>
@@ -45718,7 +45731,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A64" s="32" t="s">
         <v>288</v>
       </c>
@@ -45793,7 +45806,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A65" s="32" t="s">
         <v>288</v>
       </c>
@@ -45869,7 +45882,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A66" s="32" t="s">
         <v>288</v>
       </c>
@@ -45943,7 +45956,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A67" s="32" t="s">
         <v>288</v>
       </c>
@@ -46017,7 +46030,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A68" s="32" t="s">
         <v>288</v>
       </c>
@@ -46092,7 +46105,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A69" s="32" t="s">
         <v>288</v>
       </c>
@@ -46165,7 +46178,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A70" s="32" t="s">
         <v>288</v>
       </c>
@@ -46240,7 +46253,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A71" s="32" t="s">
         <v>288</v>
       </c>
@@ -46315,7 +46328,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A72" s="32" t="s">
         <v>288</v>
       </c>
@@ -46390,7 +46403,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A73" s="32" t="s">
         <v>288</v>
       </c>
@@ -46468,7 +46481,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A74" s="32" t="s">
         <v>288</v>
       </c>
@@ -46546,7 +46559,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A75" s="32" t="s">
         <v>288</v>
       </c>
@@ -46624,7 +46637,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A76" s="32" t="s">
         <v>288</v>
       </c>
@@ -46699,7 +46712,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="77" spans="1:23">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A77" s="32" t="s">
         <v>288</v>
       </c>
@@ -46773,7 +46786,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A78" s="70" t="s">
         <v>484</v>
       </c>
@@ -46847,7 +46860,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A79" s="74" t="s">
         <v>484</v>
       </c>
@@ -46923,7 +46936,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A80" s="74" t="s">
         <v>484</v>
       </c>
@@ -46999,7 +47012,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="81" spans="1:23">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A81" s="74" t="s">
         <v>484</v>
       </c>
@@ -47075,7 +47088,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="82" spans="1:23">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A82" s="74" t="s">
         <v>484</v>
       </c>
@@ -47151,7 +47164,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A83" s="74" t="s">
         <v>484</v>
       </c>
@@ -47227,7 +47240,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="84" spans="1:23">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A84" s="74" t="s">
         <v>484</v>
       </c>
@@ -47303,7 +47316,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="85" spans="1:23">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A85" s="74" t="s">
         <v>484</v>
       </c>
@@ -47378,7 +47391,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="86" spans="1:23">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A86" s="74" t="s">
         <v>484</v>
       </c>
@@ -47453,7 +47466,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A87" s="74" t="s">
         <v>484</v>
       </c>
@@ -47529,7 +47542,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="88" spans="1:23">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A88" s="74" t="s">
         <v>484</v>
       </c>
@@ -47607,7 +47620,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="89" spans="1:23">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A89" s="74" t="s">
         <v>484</v>
       </c>
@@ -47684,7 +47697,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="90" spans="1:23">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A90" s="74" t="s">
         <v>484</v>
       </c>
@@ -47762,7 +47775,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="91" spans="1:23">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A91" s="74" t="s">
         <v>484</v>
       </c>
@@ -47839,7 +47852,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="92" spans="1:23">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A92" s="74" t="s">
         <v>484</v>
       </c>
@@ -47915,7 +47928,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="93" spans="1:23">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A93" s="74" t="s">
         <v>484</v>
       </c>
@@ -47987,7 +48000,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="94" spans="1:23">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A94" s="74" t="s">
         <v>484</v>
       </c>
@@ -48059,7 +48072,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="95" spans="1:23">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A95" s="74" t="s">
         <v>484</v>
       </c>
@@ -48134,7 +48147,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="96" spans="1:23">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A96" s="74" t="s">
         <v>484</v>
       </c>
@@ -48206,7 +48219,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="97" spans="1:23">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A97" s="74" t="s">
         <v>484</v>
       </c>
@@ -48282,7 +48295,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="98" spans="1:23">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A98" s="74" t="s">
         <v>484</v>
       </c>
@@ -48358,7 +48371,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="99" spans="1:23">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A99" s="74" t="s">
         <v>484</v>
       </c>
@@ -48431,7 +48444,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="100" spans="1:23">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A100" s="74" t="s">
         <v>484</v>
       </c>
@@ -48507,7 +48520,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="101" spans="1:23">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A101" s="70" t="s">
         <v>484</v>
       </c>
@@ -48582,7 +48595,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="102" spans="1:23">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A102" s="74" t="s">
         <v>484</v>
       </c>
@@ -48656,7 +48669,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="103" spans="1:23">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A103" s="74" t="s">
         <v>484</v>
       </c>
@@ -48727,7 +48740,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="104" spans="1:23">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A104" s="74" t="s">
         <v>484</v>
       </c>
@@ -48798,7 +48811,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="105" spans="1:23">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A105" s="74" t="s">
         <v>484</v>
       </c>
@@ -48871,7 +48884,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="106" spans="1:23">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A106" s="70" t="s">
         <v>484</v>
       </c>
@@ -48945,7 +48958,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="107" spans="1:23">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A107" s="74" t="s">
         <v>484</v>
       </c>
@@ -49019,7 +49032,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="108" spans="1:23">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A108" s="74" t="s">
         <v>484</v>
       </c>
@@ -49094,7 +49107,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="109" spans="1:23">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A109" s="74" t="s">
         <v>484</v>
       </c>
@@ -49170,7 +49183,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="110" spans="1:23">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A110" s="74" t="s">
         <v>484</v>
       </c>
@@ -49244,7 +49257,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="111" spans="1:23">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A111" s="74" t="s">
         <v>484</v>
       </c>
@@ -49319,7 +49332,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="112" spans="1:23">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A112" s="74" t="s">
         <v>484</v>
       </c>
@@ -49393,7 +49406,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="113" spans="1:23">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A113" s="74" t="s">
         <v>484</v>
       </c>
@@ -49466,7 +49479,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="114" spans="1:23">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A114" s="74" t="s">
         <v>484</v>
       </c>
@@ -49539,7 +49552,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="115" spans="1:23">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A115" s="74" t="s">
         <v>484</v>
       </c>
@@ -49613,7 +49626,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="116" spans="1:23">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A116" s="74" t="s">
         <v>484</v>
       </c>
@@ -49687,7 +49700,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="117" spans="1:23">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A117" s="74" t="s">
         <v>484</v>
       </c>
@@ -49762,7 +49775,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="118" spans="1:23">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A118" s="74" t="s">
         <v>484</v>
       </c>
@@ -49836,7 +49849,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="119" spans="1:23">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A119" s="74" t="s">
         <v>484</v>
       </c>
@@ -49910,7 +49923,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="120" spans="1:23">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A120" s="74" t="s">
         <v>484</v>
       </c>
@@ -49984,7 +49997,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="121" spans="1:23">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A121" s="74" t="s">
         <v>484</v>
       </c>
@@ -50061,7 +50074,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="122" spans="1:23">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A122" s="74" t="s">
         <v>484</v>
       </c>
@@ -50135,7 +50148,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="123" spans="1:23">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A123" s="74" t="s">
         <v>484</v>
       </c>
@@ -50210,7 +50223,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="124" spans="1:23">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A124" s="74" t="s">
         <v>484</v>
       </c>
@@ -50287,7 +50300,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="125" spans="1:23">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A125" s="74" t="s">
         <v>484</v>
       </c>
@@ -50363,7 +50376,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="126" spans="1:23">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A126" s="74" t="s">
         <v>484</v>
       </c>
@@ -50440,7 +50453,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="127" spans="1:23">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A127" s="74" t="s">
         <v>484</v>
       </c>
@@ -50517,7 +50530,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="128" spans="1:23">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A128" s="74" t="s">
         <v>484</v>
       </c>
@@ -50592,7 +50605,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="129" spans="1:23">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A129" s="74" t="s">
         <v>484</v>
       </c>
@@ -50668,7 +50681,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="130" spans="1:23">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A130" s="70" t="s">
         <v>484</v>
       </c>
@@ -50744,7 +50757,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="131" spans="1:23">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A131" s="74" t="s">
         <v>484</v>
       </c>
@@ -50819,7 +50832,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="132" spans="1:23">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A132" s="74" t="s">
         <v>484</v>
       </c>
@@ -50896,7 +50909,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="133" spans="1:23">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A133" s="70" t="s">
         <v>484</v>
       </c>
@@ -50974,7 +50987,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="134" spans="1:23">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A134" s="74" t="s">
         <v>484</v>
       </c>
@@ -51051,7 +51064,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="135" spans="1:23">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A135" s="74" t="s">
         <v>484</v>
       </c>
@@ -51129,7 +51142,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="136" spans="1:23">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A136" s="74" t="s">
         <v>484</v>
       </c>
@@ -51207,7 +51220,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="137" spans="1:23">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A137" s="74" t="s">
         <v>484</v>
       </c>
@@ -51283,7 +51296,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="138" spans="1:23">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A138" s="74" t="s">
         <v>484</v>
       </c>
@@ -51356,7 +51369,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="139" spans="1:23">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A139" s="74" t="s">
         <v>484</v>
       </c>
@@ -51432,7 +51445,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="140" spans="1:23">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A140" s="74" t="s">
         <v>484</v>
       </c>
@@ -51506,7 +51519,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="141" spans="1:23">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A141" s="74" t="s">
         <v>0</v>
       </c>
@@ -51582,7 +51595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:23">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A142" s="74" t="s">
         <v>0</v>
       </c>
@@ -51657,7 +51670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="1:23">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A143" s="74" t="s">
         <v>0</v>
       </c>
@@ -51731,7 +51744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="1:23">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A144" s="74" t="s">
         <v>0</v>
       </c>
@@ -51806,7 +51819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:23">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A145" s="74" t="s">
         <v>0</v>
       </c>
@@ -51879,7 +51892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:23">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A146" s="74" t="s">
         <v>0</v>
       </c>
@@ -51953,7 +51966,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:23">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A147" s="74" t="s">
         <v>0</v>
       </c>
@@ -52025,7 +52038,7 @@
       </c>
       <c r="W147" s="91"/>
     </row>
-    <row r="148" spans="1:23">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A148" s="74" t="s">
         <v>0</v>
       </c>
@@ -52097,7 +52110,7 @@
       </c>
       <c r="W148" s="106"/>
     </row>
-    <row r="149" spans="1:23">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A149" s="74" t="s">
         <v>0</v>
       </c>
@@ -52170,7 +52183,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="150" spans="1:23">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A150" s="74" t="s">
         <v>0</v>
       </c>
@@ -52243,7 +52256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="151" spans="1:23">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A151" s="74" t="s">
         <v>0</v>
       </c>
@@ -52315,7 +52328,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="152" spans="1:23">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A152" s="74" t="s">
         <v>0</v>
       </c>
@@ -52386,7 +52399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="153" spans="1:23">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A153" s="74" t="s">
         <v>0</v>
       </c>
@@ -52461,7 +52474,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="154" spans="1:23">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A154" s="74" t="s">
         <v>0</v>
       </c>
@@ -52536,7 +52549,7 @@
         <v>39845</v>
       </c>
     </row>
-    <row r="155" spans="1:23">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A155" s="74" t="s">
         <v>0</v>
       </c>
@@ -52603,7 +52616,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="156" spans="1:23">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A156" s="74" t="s">
         <v>0</v>
       </c>
@@ -52677,7 +52690,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="157" spans="1:23">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A157" s="74" t="s">
         <v>0</v>
       </c>
@@ -52749,7 +52762,7 @@
       </c>
       <c r="W157" s="20"/>
     </row>
-    <row r="158" spans="1:23">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A158" s="74" t="s">
         <v>0</v>
       </c>
@@ -52824,7 +52837,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="159" spans="1:23">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A159" s="74" t="s">
         <v>0</v>
       </c>
@@ -52891,7 +52904,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="160" spans="1:23">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A160" s="74" t="s">
         <v>0</v>
       </c>
@@ -52958,7 +52971,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="161" spans="1:23">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A161" s="74" t="s">
         <v>0</v>
       </c>
@@ -53025,7 +53038,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="162" spans="1:23">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A162" s="74" t="s">
         <v>0</v>
       </c>
@@ -53097,7 +53110,7 @@
       </c>
       <c r="W162" s="14"/>
     </row>
-    <row r="163" spans="1:23">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A163" s="74" t="s">
         <v>0</v>
       </c>
@@ -53171,7 +53184,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="164" spans="1:23">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A164" s="74" t="s">
         <v>0</v>
       </c>
@@ -53243,7 +53256,7 @@
       </c>
       <c r="W164" s="22"/>
     </row>
-    <row r="165" spans="1:23">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A165" s="74" t="s">
         <v>0</v>
       </c>
@@ -53308,7 +53321,7 @@
       </c>
       <c r="W165" s="140"/>
     </row>
-    <row r="166" spans="1:23">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A166" s="74" t="s">
         <v>0</v>
       </c>
@@ -53382,7 +53395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="167" spans="1:23">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A167" s="74" t="s">
         <v>0</v>
       </c>
@@ -53457,7 +53470,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:23">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A168" s="74" t="s">
         <v>0</v>
       </c>
@@ -53528,7 +53541,7 @@
       </c>
       <c r="W168" s="17"/>
     </row>
-    <row r="169" spans="1:23">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A169" s="74" t="s">
         <v>0</v>
       </c>
@@ -53596,7 +53609,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:23">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A170" s="74" t="s">
         <v>0</v>
       </c>
@@ -53664,7 +53677,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="13" thickBot="1">
+    <row r="171" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A171" s="74" t="s">
         <v>0</v>
       </c>
@@ -53731,7 +53744,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="13" thickBot="1">
+    <row r="172" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A172" s="74" t="s">
         <v>0</v>
       </c>
@@ -53807,7 +53820,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="13" thickBot="1">
+    <row r="173" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A173" s="74" t="s">
         <v>0</v>
       </c>
@@ -53883,7 +53896,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="13" thickBot="1">
+    <row r="174" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A174" s="74" t="s">
         <v>0</v>
       </c>
@@ -53959,7 +53972,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="13" thickBot="1">
+    <row r="175" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A175" s="74" t="s">
         <v>0</v>
       </c>
@@ -54035,7 +54048,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="176" spans="1:23">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A176" s="74" t="s">
         <v>0</v>
       </c>
@@ -54110,7 +54123,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:23">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A177" s="74" t="s">
         <v>0</v>
       </c>
@@ -54186,7 +54199,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="178" spans="1:23">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A178" s="74" t="s">
         <v>0</v>
       </c>
@@ -54259,7 +54272,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="179" spans="1:23">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A179" s="74" t="s">
         <v>0</v>
       </c>
@@ -54335,7 +54348,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="180" spans="1:23">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A180" s="74" t="s">
         <v>0</v>
       </c>
@@ -54404,7 +54417,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="181" spans="1:23">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A181" s="74" t="s">
         <v>0</v>
       </c>
@@ -54477,7 +54490,7 @@
       </c>
       <c r="W181" s="190"/>
     </row>
-    <row r="182" spans="1:23">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A182" s="74" t="s">
         <v>0</v>
       </c>
@@ -54551,7 +54564,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="183" spans="1:23">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A183" s="74" t="s">
         <v>0</v>
       </c>
@@ -54617,7 +54630,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="184" spans="1:23">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A184" s="74" t="s">
         <v>0</v>
       </c>
@@ -54691,7 +54704,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="185" spans="1:23">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A185" s="74" t="s">
         <v>0</v>
       </c>
@@ -54766,7 +54779,7 @@
       </c>
       <c r="W185" s="206"/>
     </row>
-    <row r="186" spans="1:23">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A186" s="74" t="s">
         <v>0</v>
       </c>
@@ -54837,7 +54850,7 @@
       </c>
       <c r="W186" s="211"/>
     </row>
-    <row r="187" spans="1:23">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A187" s="74" t="s">
         <v>0</v>
       </c>
@@ -54907,7 +54920,7 @@
       </c>
       <c r="W187" s="171"/>
     </row>
-    <row r="188" spans="1:23">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A188" s="74" t="s">
         <v>0</v>
       </c>
@@ -54978,7 +54991,7 @@
       </c>
       <c r="W188" s="211"/>
     </row>
-    <row r="189" spans="1:23">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A189" s="74" t="s">
         <v>0</v>
       </c>
@@ -55051,7 +55064,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="190" spans="1:23">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A190" s="74" t="s">
         <v>0</v>
       </c>
@@ -55124,7 +55137,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="191" spans="1:23">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A191" s="74" t="s">
         <v>0</v>
       </c>
@@ -55197,7 +55210,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="192" spans="1:23">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A192" s="32" t="s">
         <v>1</v>
       </c>
@@ -55269,7 +55282,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="193" spans="1:23">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A193" s="32" t="s">
         <v>1</v>
       </c>
@@ -55342,7 +55355,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="194" spans="1:23">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A194" s="224" t="s">
         <v>1</v>
       </c>
@@ -55415,7 +55428,7 @@
       </c>
       <c r="W194" s="225"/>
     </row>
-    <row r="195" spans="1:23">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A195" s="32" t="s">
         <v>1</v>
       </c>
@@ -55486,7 +55499,7 @@
       </c>
       <c r="W195" s="67"/>
     </row>
-    <row r="196" spans="1:23">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A196" s="32" t="s">
         <v>1</v>
       </c>
@@ -55562,7 +55575,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="197" spans="1:23">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A197" s="32" t="s">
         <v>1</v>
       </c>
@@ -55636,7 +55649,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="198" spans="1:23">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A198" s="32" t="s">
         <v>1</v>
       </c>
@@ -55711,7 +55724,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="199" spans="1:23">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A199" s="32" t="s">
         <v>1</v>
       </c>
@@ -55785,7 +55798,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="200" spans="1:23">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A200" s="32" t="s">
         <v>1</v>
       </c>
@@ -55861,7 +55874,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="201" spans="1:23">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A201" s="224" t="s">
         <v>1</v>
       </c>
@@ -55936,7 +55949,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="202" spans="1:23">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A202" s="32" t="s">
         <v>1</v>
       </c>
@@ -56012,7 +56025,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="203" spans="1:23">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A203" s="32" t="s">
         <v>1</v>
       </c>
@@ -56086,7 +56099,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="204" spans="1:23">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A204" s="32" t="s">
         <v>1</v>
       </c>
@@ -56160,7 +56173,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="205" spans="1:23">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A205" s="32" t="s">
         <v>1</v>
       </c>
@@ -56235,7 +56248,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="206" spans="1:23">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A206" s="32" t="s">
         <v>1</v>
       </c>
@@ -56310,7 +56323,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="207" spans="1:23">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A207" s="32" t="s">
         <v>1</v>
       </c>
@@ -56383,7 +56396,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="208" spans="1:23">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A208" s="32" t="s">
         <v>1</v>
       </c>
@@ -56456,7 +56469,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="209" spans="1:23">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A209" s="32" t="s">
         <v>1</v>
       </c>
@@ -56529,7 +56542,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="210" spans="1:23">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A210" s="32" t="s">
         <v>1</v>
       </c>
@@ -56603,7 +56616,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="211" spans="1:23">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A211" s="32" t="s">
         <v>1</v>
       </c>
@@ -56677,7 +56690,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="212" spans="1:23">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A212" s="32" t="s">
         <v>1</v>
       </c>
@@ -56751,7 +56764,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="213" spans="1:23">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A213" s="32" t="s">
         <v>1</v>
       </c>
@@ -56825,7 +56838,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="214" spans="1:23">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A214" s="32" t="s">
         <v>1</v>
       </c>
@@ -56899,7 +56912,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="215" spans="1:23">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A215" s="32" t="s">
         <v>1</v>
       </c>
@@ -56973,7 +56986,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="216" spans="1:23">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A216" s="32" t="s">
         <v>1</v>
       </c>
@@ -57047,7 +57060,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="217" spans="1:23">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A217" s="32" t="s">
         <v>1</v>
       </c>
@@ -57119,7 +57132,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="218" spans="1:23">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A218" s="32" t="s">
         <v>1</v>
       </c>
@@ -57193,7 +57206,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="219" spans="1:23">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A219" s="32" t="s">
         <v>1</v>
       </c>
@@ -57267,7 +57280,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="220" spans="1:23">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A220" s="32" t="s">
         <v>1</v>
       </c>
@@ -57340,7 +57353,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="221" spans="1:23">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A221" s="32" t="s">
         <v>1</v>
       </c>
@@ -57413,7 +57426,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="222" spans="1:23">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A222" s="32" t="s">
         <v>1</v>
       </c>
@@ -57489,7 +57502,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="223" spans="1:23">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A223" s="32" t="s">
         <v>1</v>
       </c>
@@ -57563,7 +57576,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="224" spans="1:23">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A224" s="32" t="s">
         <v>1</v>
       </c>
@@ -57637,7 +57650,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="225" spans="1:23">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A225" s="32" t="s">
         <v>1</v>
       </c>
@@ -57711,7 +57724,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="226" spans="1:23">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A226" s="32" t="s">
         <v>1</v>
       </c>
@@ -57787,7 +57800,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="227" spans="1:23">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A227" s="32" t="s">
         <v>1</v>
       </c>
@@ -57861,7 +57874,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="228" spans="1:23">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A228" s="32" t="s">
         <v>1</v>
       </c>
@@ -57934,7 +57947,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="229" spans="1:23">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A229" s="32" t="s">
         <v>1</v>
       </c>
@@ -58007,7 +58020,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="230" spans="1:23">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A230" s="32" t="s">
         <v>1</v>
       </c>
@@ -58082,7 +58095,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="231" spans="1:23">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A231" s="32" t="s">
         <v>1</v>
       </c>
@@ -58157,7 +58170,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="232" spans="1:23">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A232" s="32" t="s">
         <v>1</v>
       </c>
@@ -58232,7 +58245,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="233" spans="1:23">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A233" s="32" t="s">
         <v>1</v>
       </c>
@@ -58305,7 +58318,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="234" spans="1:23">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A234" s="32" t="s">
         <v>1</v>
       </c>
@@ -58378,7 +58391,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="235" spans="1:23">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A235" s="32" t="s">
         <v>1</v>
       </c>
@@ -58451,7 +58464,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="236" spans="1:23">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A236" s="32" t="s">
         <v>1</v>
       </c>
@@ -58524,7 +58537,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="237" spans="1:23">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A237" s="32" t="s">
         <v>1</v>
       </c>
@@ -58598,7 +58611,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="238" spans="1:23">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A238" s="32" t="s">
         <v>1</v>
       </c>
@@ -58672,7 +58685,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="239" spans="1:23">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A239" s="32" t="s">
         <v>1</v>
       </c>
@@ -58746,7 +58759,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="240" spans="1:23">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A240" s="32" t="s">
         <v>1</v>
       </c>
@@ -58821,7 +58834,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="241" spans="1:23">
+    <row r="241" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A241" s="32" t="s">
         <v>1</v>
       </c>
@@ -58896,7 +58909,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="242" spans="1:23">
+    <row r="242" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A242" s="32" t="s">
         <v>1</v>
       </c>
@@ -58970,7 +58983,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="243" spans="1:23">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A243" s="32" t="s">
         <v>1</v>
       </c>
@@ -59043,7 +59056,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="244" spans="1:23">
+    <row r="244" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A244" s="32" t="s">
         <v>1</v>
       </c>
@@ -59116,7 +59129,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="245" spans="1:23">
+    <row r="245" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A245" s="32" t="s">
         <v>1</v>
       </c>
@@ -59191,7 +59204,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="246" spans="1:23">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A246" s="243" t="s">
         <v>651</v>
       </c>
@@ -59263,7 +59276,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="247" spans="1:23">
+    <row r="247" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A247" s="243" t="s">
         <v>651</v>
       </c>
@@ -59334,7 +59347,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="248" spans="1:23">
+    <row r="248" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A248" s="243" t="s">
         <v>651</v>
       </c>
@@ -59407,7 +59420,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="249" spans="1:23">
+    <row r="249" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A249" s="243" t="s">
         <v>651</v>
       </c>
@@ -59481,7 +59494,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="250" spans="1:23">
+    <row r="250" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A250" s="243" t="s">
         <v>651</v>
       </c>
@@ -59559,7 +59572,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="251" spans="1:23">
+    <row r="251" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A251" s="243" t="s">
         <v>651</v>
       </c>
@@ -59634,7 +59647,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="252" spans="1:23">
+    <row r="252" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A252" s="243" t="s">
         <v>651</v>
       </c>
@@ -59709,7 +59722,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="253" spans="1:23">
+    <row r="253" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A253" s="243" t="s">
         <v>651</v>
       </c>
@@ -59779,7 +59792,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="254" spans="1:23">
+    <row r="254" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A254" s="243" t="s">
         <v>651</v>
       </c>
@@ -59850,7 +59863,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="255" spans="1:23">
+    <row r="255" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A255" s="243" t="s">
         <v>651</v>
       </c>
@@ -59926,7 +59939,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="256" spans="1:23">
+    <row r="256" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A256" s="243" t="s">
         <v>651</v>
       </c>
@@ -60002,7 +60015,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="257" spans="1:23">
+    <row r="257" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A257" s="243" t="s">
         <v>651</v>
       </c>
@@ -60076,7 +60089,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="258" spans="1:23">
+    <row r="258" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A258" s="243" t="s">
         <v>651</v>
       </c>
@@ -60151,7 +60164,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="259" spans="1:23">
+    <row r="259" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A259" s="243" t="s">
         <v>651</v>
       </c>
@@ -60227,7 +60240,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="260" spans="1:23">
+    <row r="260" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A260" s="243" t="s">
         <v>651</v>
       </c>
@@ -60298,7 +60311,7 @@
       <c r="V260" s="19"/>
       <c r="W260" s="19"/>
     </row>
-    <row r="261" spans="1:23">
+    <row r="261" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A261" s="243" t="s">
         <v>651</v>
       </c>
@@ -60374,7 +60387,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="262" spans="1:23">
+    <row r="262" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A262" s="243" t="s">
         <v>651</v>
       </c>
@@ -60449,7 +60462,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="263" spans="1:23">
+    <row r="263" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A263" s="243" t="s">
         <v>651</v>
       </c>
@@ -60523,7 +60536,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="264" spans="1:23">
+    <row r="264" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A264" s="243" t="s">
         <v>651</v>
       </c>
@@ -60598,7 +60611,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="265" spans="1:23">
+    <row r="265" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A265" s="243" t="s">
         <v>651</v>
       </c>
@@ -60671,7 +60684,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="266" spans="1:23">
+    <row r="266" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A266" s="243" t="s">
         <v>651</v>
       </c>
@@ -60743,7 +60756,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="267" spans="1:23">
+    <row r="267" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A267" s="243" t="s">
         <v>651</v>
       </c>
@@ -60817,7 +60830,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="268" spans="1:23">
+    <row r="268" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A268" s="243" t="s">
         <v>651</v>
       </c>
@@ -60892,7 +60905,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="269" spans="1:23">
+    <row r="269" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A269" s="243" t="s">
         <v>651</v>
       </c>
@@ -60967,7 +60980,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="270" spans="1:23">
+    <row r="270" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A270" s="243" t="s">
         <v>651</v>
       </c>
@@ -61041,7 +61054,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="271" spans="1:23">
+    <row r="271" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A271" s="243" t="s">
         <v>651</v>
       </c>
@@ -61116,7 +61129,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="272" spans="1:23">
+    <row r="272" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A272" s="243" t="s">
         <v>651</v>
       </c>
@@ -61191,7 +61204,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="273" spans="1:23">
+    <row r="273" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A273" s="243" t="s">
         <v>651</v>
       </c>
@@ -61265,7 +61278,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="274" spans="1:23">
+    <row r="274" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A274" s="243" t="s">
         <v>651</v>
       </c>
@@ -61338,7 +61351,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="275" spans="1:23">
+    <row r="275" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A275" s="243" t="s">
         <v>651</v>
       </c>
@@ -61409,7 +61422,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="276" spans="1:23">
+    <row r="276" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A276" s="243" t="s">
         <v>651</v>
       </c>
@@ -61482,7 +61495,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="277" spans="1:23">
+    <row r="277" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A277" s="243" t="s">
         <v>651</v>
       </c>
@@ -61552,7 +61565,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="278" spans="1:23">
+    <row r="278" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A278" s="243" t="s">
         <v>651</v>
       </c>
@@ -61624,7 +61637,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="279" spans="1:23">
+    <row r="279" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A279" s="243" t="s">
         <v>651</v>
       </c>
@@ -61699,7 +61712,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="280" spans="1:23">
+    <row r="280" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A280" s="243" t="s">
         <v>651</v>
       </c>
@@ -61772,7 +61785,7 @@
       </c>
       <c r="W280" s="19"/>
     </row>
-    <row r="281" spans="1:23">
+    <row r="281" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A281" s="243" t="s">
         <v>651</v>
       </c>
@@ -61843,7 +61856,7 @@
       </c>
       <c r="W281" s="19"/>
     </row>
-    <row r="282" spans="1:23">
+    <row r="282" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A282" s="243" t="s">
         <v>651</v>
       </c>
@@ -61913,7 +61926,7 @@
       <c r="V282" s="19"/>
       <c r="W282" s="19"/>
     </row>
-    <row r="283" spans="1:23">
+    <row r="283" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A283" s="243" t="s">
         <v>651</v>
       </c>
@@ -61988,7 +62001,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="284" spans="1:23">
+    <row r="284" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A284" s="243" t="s">
         <v>651</v>
       </c>
@@ -62061,7 +62074,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="285" spans="1:23">
+    <row r="285" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A285" s="243" t="s">
         <v>651</v>
       </c>
@@ -62135,7 +62148,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="286" spans="1:23">
+    <row r="286" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A286" s="243" t="s">
         <v>651</v>
       </c>
@@ -62208,7 +62221,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="287" spans="1:23">
+    <row r="287" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A287" s="243" t="s">
         <v>651</v>
       </c>
@@ -62280,7 +62293,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="288" spans="1:23">
+    <row r="288" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A288" s="254" t="s">
         <v>767</v>
       </c>
@@ -62354,7 +62367,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="289" spans="1:23">
+    <row r="289" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A289" s="254" t="s">
         <v>767</v>
       </c>
@@ -62430,7 +62443,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="290" spans="1:23">
+    <row r="290" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A290" s="254" t="s">
         <v>767</v>
       </c>
@@ -62502,7 +62515,7 @@
       </c>
       <c r="W290" s="9"/>
     </row>
-    <row r="291" spans="1:23">
+    <row r="291" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A291" s="254" t="s">
         <v>767</v>
       </c>
@@ -62577,7 +62590,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="292" spans="1:23">
+    <row r="292" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A292" s="254" t="s">
         <v>767</v>
       </c>
@@ -62649,7 +62662,7 @@
       </c>
       <c r="W292" s="19"/>
     </row>
-    <row r="293" spans="1:23">
+    <row r="293" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A293" s="254" t="s">
         <v>767</v>
       </c>
@@ -62721,7 +62734,7 @@
       </c>
       <c r="W293" s="19"/>
     </row>
-    <row r="294" spans="1:23">
+    <row r="294" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A294" s="254" t="s">
         <v>767</v>
       </c>
@@ -62793,7 +62806,7 @@
       </c>
       <c r="W294" s="9"/>
     </row>
-    <row r="295" spans="1:23">
+    <row r="295" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A295" s="254" t="s">
         <v>767</v>
       </c>
@@ -62865,7 +62878,7 @@
       </c>
       <c r="W295" s="9"/>
     </row>
-    <row r="296" spans="1:23">
+    <row r="296" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A296" s="254" t="s">
         <v>767</v>
       </c>
@@ -62937,7 +62950,7 @@
       </c>
       <c r="W296" s="9"/>
     </row>
-    <row r="297" spans="1:23">
+    <row r="297" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A297" s="254" t="s">
         <v>767</v>
       </c>
@@ -63013,7 +63026,7 @@
       </c>
       <c r="W297" s="9"/>
     </row>
-    <row r="298" spans="1:23">
+    <row r="298" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A298" s="254" t="s">
         <v>767</v>
       </c>
@@ -63089,7 +63102,7 @@
       </c>
       <c r="W298" s="9"/>
     </row>
-    <row r="299" spans="1:23">
+    <row r="299" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A299" s="254" t="s">
         <v>767</v>
       </c>
@@ -63162,7 +63175,7 @@
       </c>
       <c r="W299" s="9"/>
     </row>
-    <row r="300" spans="1:23">
+    <row r="300" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A300" s="254" t="s">
         <v>767</v>
       </c>
@@ -63235,7 +63248,7 @@
       </c>
       <c r="W300" s="9"/>
     </row>
-    <row r="301" spans="1:23">
+    <row r="301" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A301" s="254" t="s">
         <v>767</v>
       </c>
@@ -63308,7 +63321,7 @@
       </c>
       <c r="W301" s="9"/>
     </row>
-    <row r="302" spans="1:23">
+    <row r="302" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A302" s="254" t="s">
         <v>767</v>
       </c>
@@ -63381,7 +63394,7 @@
       </c>
       <c r="W302" s="9"/>
     </row>
-    <row r="303" spans="1:23">
+    <row r="303" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A303" s="254" t="s">
         <v>767</v>
       </c>
@@ -63454,7 +63467,7 @@
       </c>
       <c r="W303" s="9"/>
     </row>
-    <row r="304" spans="1:23">
+    <row r="304" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A304" s="254" t="s">
         <v>767</v>
       </c>
@@ -63528,7 +63541,7 @@
       </c>
       <c r="W304" s="9"/>
     </row>
-    <row r="305" spans="1:23">
+    <row r="305" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A305" s="254" t="s">
         <v>767</v>
       </c>
@@ -63602,7 +63615,7 @@
       </c>
       <c r="W305" s="9"/>
     </row>
-    <row r="306" spans="1:23">
+    <row r="306" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A306" s="254" t="s">
         <v>767</v>
       </c>
@@ -63673,7 +63686,7 @@
       </c>
       <c r="W306" s="19"/>
     </row>
-    <row r="307" spans="1:23">
+    <row r="307" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A307" s="254" t="s">
         <v>767</v>
       </c>
@@ -63744,7 +63757,7 @@
       </c>
       <c r="W307" s="19"/>
     </row>
-    <row r="308" spans="1:23">
+    <row r="308" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A308" s="254" t="s">
         <v>767</v>
       </c>
@@ -63815,7 +63828,7 @@
       </c>
       <c r="W308" s="19"/>
     </row>
-    <row r="309" spans="1:23">
+    <row r="309" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A309" s="299" t="s">
         <v>767</v>
       </c>
@@ -63889,7 +63902,7 @@
       </c>
       <c r="W309" s="302"/>
     </row>
-    <row r="310" spans="1:23">
+    <row r="310" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A310" s="299" t="s">
         <v>767</v>
       </c>
@@ -63962,7 +63975,7 @@
       </c>
       <c r="W310" s="302"/>
     </row>
-    <row r="311" spans="1:23">
+    <row r="311" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A311" s="299" t="s">
         <v>767</v>
       </c>
@@ -64035,7 +64048,7 @@
       </c>
       <c r="W311" s="302"/>
     </row>
-    <row r="312" spans="1:23">
+    <row r="312" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A312" s="299" t="s">
         <v>767</v>
       </c>
@@ -64106,7 +64119,7 @@
       </c>
       <c r="W312" s="302"/>
     </row>
-    <row r="313" spans="1:23">
+    <row r="313" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A313" s="254" t="s">
         <v>767</v>
       </c>
@@ -64179,7 +64192,7 @@
       </c>
       <c r="W313" s="19"/>
     </row>
-    <row r="314" spans="1:23">
+    <row r="314" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A314" s="254" t="s">
         <v>767</v>
       </c>
@@ -64252,7 +64265,7 @@
       </c>
       <c r="W314" s="19"/>
     </row>
-    <row r="315" spans="1:23">
+    <row r="315" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A315" s="254" t="s">
         <v>767</v>
       </c>
@@ -64326,7 +64339,7 @@
       </c>
       <c r="W315" s="19"/>
     </row>
-    <row r="316" spans="1:23">
+    <row r="316" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A316" s="254" t="s">
         <v>767</v>
       </c>
@@ -64400,7 +64413,7 @@
       </c>
       <c r="W316" s="19"/>
     </row>
-    <row r="317" spans="1:23">
+    <row r="317" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A317" s="254" t="s">
         <v>767</v>
       </c>
@@ -64474,7 +64487,7 @@
       </c>
       <c r="W317" s="19"/>
     </row>
-    <row r="318" spans="1:23">
+    <row r="318" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A318" s="254" t="s">
         <v>767</v>
       </c>
@@ -64549,7 +64562,7 @@
       </c>
       <c r="W318" s="19"/>
     </row>
-    <row r="319" spans="1:23">
+    <row r="319" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A319" s="254" t="s">
         <v>767</v>
       </c>
@@ -64624,7 +64637,7 @@
       </c>
       <c r="W319" s="19"/>
     </row>
-    <row r="320" spans="1:23">
+    <row r="320" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A320" s="254" t="s">
         <v>767</v>
       </c>
@@ -64696,7 +64709,7 @@
       </c>
       <c r="W320" s="19"/>
     </row>
-    <row r="321" spans="1:23">
+    <row r="321" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A321" s="254" t="s">
         <v>767</v>
       </c>
@@ -64768,7 +64781,7 @@
       </c>
       <c r="W321" s="19"/>
     </row>
-    <row r="322" spans="1:23">
+    <row r="322" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A322" s="254" t="s">
         <v>767</v>
       </c>
@@ -64839,7 +64852,7 @@
       </c>
       <c r="W322" s="19"/>
     </row>
-    <row r="323" spans="1:23">
+    <row r="323" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A323" s="254" t="s">
         <v>767</v>
       </c>
@@ -64914,7 +64927,7 @@
       </c>
       <c r="W323" s="19"/>
     </row>
-    <row r="324" spans="1:23">
+    <row r="324" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A324" s="254" t="s">
         <v>767</v>
       </c>
@@ -64986,7 +64999,7 @@
       </c>
       <c r="W324" s="19"/>
     </row>
-    <row r="325" spans="1:23">
+    <row r="325" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A325" s="254" t="s">
         <v>767</v>
       </c>
@@ -65057,7 +65070,7 @@
       </c>
       <c r="W325" s="19"/>
     </row>
-    <row r="326" spans="1:23">
+    <row r="326" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A326" s="254" t="s">
         <v>767</v>
       </c>
@@ -65130,7 +65143,7 @@
       </c>
       <c r="W326" s="19"/>
     </row>
-    <row r="327" spans="1:23">
+    <row r="327" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A327" s="299" t="s">
         <v>767</v>
       </c>
@@ -65202,7 +65215,7 @@
       </c>
       <c r="W327" s="302"/>
     </row>
-    <row r="328" spans="1:23">
+    <row r="328" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A328" s="299" t="s">
         <v>767</v>
       </c>
@@ -65275,7 +65288,7 @@
       </c>
       <c r="W328" s="302"/>
     </row>
-    <row r="329" spans="1:23">
+    <row r="329" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A329" s="254" t="s">
         <v>767</v>
       </c>
@@ -65347,7 +65360,7 @@
       </c>
       <c r="W329" s="19"/>
     </row>
-    <row r="330" spans="1:23">
+    <row r="330" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A330" s="305" t="s">
         <v>767</v>
       </c>
@@ -65420,7 +65433,7 @@
       </c>
       <c r="W330" s="297"/>
     </row>
-    <row r="331" spans="1:23">
+    <row r="331" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A331" s="254" t="s">
         <v>767</v>
       </c>
@@ -65495,7 +65508,7 @@
       </c>
       <c r="W331" s="19"/>
     </row>
-    <row r="332" spans="1:23">
+    <row r="332" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A332" s="254" t="s">
         <v>767</v>
       </c>
@@ -65568,7 +65581,7 @@
       </c>
       <c r="W332" s="19"/>
     </row>
-    <row r="333" spans="1:23">
+    <row r="333" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A333" s="254" t="s">
         <v>767</v>
       </c>
@@ -65643,7 +65656,7 @@
       </c>
       <c r="W333" s="19"/>
     </row>
-    <row r="334" spans="1:23">
+    <row r="334" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A334" s="254" t="s">
         <v>767</v>
       </c>
@@ -65717,7 +65730,7 @@
       </c>
       <c r="W334" s="19"/>
     </row>
-    <row r="335" spans="1:23">
+    <row r="335" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A335" s="254" t="s">
         <v>767</v>
       </c>
@@ -65790,7 +65803,7 @@
       </c>
       <c r="W335" s="19"/>
     </row>
-    <row r="336" spans="1:23">
+    <row r="336" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A336" s="254" t="s">
         <v>767</v>
       </c>
@@ -65864,7 +65877,7 @@
       </c>
       <c r="W336" s="19"/>
     </row>
-    <row r="337" spans="1:23">
+    <row r="337" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A337" s="254" t="s">
         <v>767</v>
       </c>
@@ -65937,7 +65950,7 @@
       </c>
       <c r="W337" s="19"/>
     </row>
-    <row r="338" spans="1:23">
+    <row r="338" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A338" s="254" t="s">
         <v>767</v>
       </c>
@@ -66010,7 +66023,7 @@
       </c>
       <c r="W338" s="19"/>
     </row>
-    <row r="339" spans="1:23">
+    <row r="339" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A339" s="254" t="s">
         <v>767</v>
       </c>
@@ -66085,7 +66098,7 @@
       </c>
       <c r="W339" s="19"/>
     </row>
-    <row r="340" spans="1:23">
+    <row r="340" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A340" s="254" t="s">
         <v>767</v>
       </c>
@@ -66161,7 +66174,7 @@
       </c>
       <c r="W340" s="19"/>
     </row>
-    <row r="341" spans="1:23">
+    <row r="341" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A341" s="254" t="s">
         <v>767</v>
       </c>
@@ -66237,7 +66250,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="342" spans="1:23">
+    <row r="342" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A342" s="254" t="s">
         <v>767</v>
       </c>
@@ -66312,7 +66325,7 @@
       </c>
       <c r="W342" s="19"/>
     </row>
-    <row r="343" spans="1:23">
+    <row r="343" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A343" s="254" t="s">
         <v>767</v>
       </c>
@@ -66390,7 +66403,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="344" spans="1:23">
+    <row r="344" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A344" s="254" t="s">
         <v>767</v>
       </c>
@@ -66468,7 +66481,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="345" spans="1:23">
+    <row r="345" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A345" s="254" t="s">
         <v>767</v>
       </c>
@@ -66546,7 +66559,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="346" spans="1:23">
+    <row r="346" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A346" s="254" t="s">
         <v>767</v>
       </c>
@@ -66619,7 +66632,7 @@
       </c>
       <c r="W346" s="19"/>
     </row>
-    <row r="347" spans="1:23">
+    <row r="347" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A347" s="254" t="s">
         <v>767</v>
       </c>
@@ -66693,7 +66706,7 @@
       </c>
       <c r="W347" s="19"/>
     </row>
-    <row r="348" spans="1:23">
+    <row r="348" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A348" s="254" t="s">
         <v>767</v>
       </c>
@@ -66764,7 +66777,7 @@
       </c>
       <c r="W348" s="19"/>
     </row>
-    <row r="349" spans="1:23">
+    <row r="349" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A349" s="249" t="s">
         <v>767</v>
       </c>
@@ -66837,7 +66850,7 @@
       </c>
       <c r="W349" s="249"/>
     </row>
-    <row r="350" spans="1:23">
+    <row r="350" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A350" s="254" t="s">
         <v>767</v>
       </c>
@@ -66910,7 +66923,7 @@
       </c>
       <c r="W350" s="19"/>
     </row>
-    <row r="351" spans="1:23">
+    <row r="351" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A351" s="254" t="s">
         <v>767</v>
       </c>
@@ -66999,11 +67012,6 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId7"/>
   <legacyDrawing r:id="rId8"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -67011,16 +67019,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="36" t="s">
         <v>901</v>
       </c>
@@ -67028,7 +67036,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="322">
         <v>10</v>
       </c>
@@ -67036,7 +67044,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="63">
         <v>10</v>
       </c>
@@ -67044,7 +67052,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="268">
         <v>10</v>
       </c>
@@ -67052,7 +67060,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="266">
         <v>10</v>
       </c>
@@ -67060,7 +67068,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="323">
         <v>10</v>
       </c>
@@ -67068,7 +67076,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="309">
         <v>10</v>
       </c>
@@ -67076,7 +67084,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="77">
         <v>10</v>
       </c>
@@ -67084,7 +67092,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="77">
         <v>10</v>
       </c>
@@ -67092,7 +67100,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="85">
         <v>10</v>
       </c>
@@ -67100,7 +67108,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="108">
         <v>10</v>
       </c>
@@ -67108,7 +67116,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="189">
         <v>10</v>
       </c>
@@ -67116,7 +67124,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="320">
         <v>10</v>
       </c>
@@ -67124,7 +67132,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="321">
         <v>10</v>
       </c>
@@ -67135,10 +67143,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>